<commit_message>
Updates to the Assembly documentation which combines multiple former documents into one and improves clarity.
</commit_message>
<xml_diff>
--- a/Gen1/Assembly/BOM_PSC.xlsx
+++ b/Gen1/Assembly/BOM_PSC.xlsx
@@ -13,11 +13,9 @@
   </bookViews>
   <sheets>
     <sheet name="BOM_PSC" sheetId="1" r:id="rId1"/>
-    <sheet name="BOM_PWMAttenuation" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="PWMAttenuation" localSheetId="0">BOM_PSC!$A$1:$E$16</definedName>
-    <definedName name="PWMAttenuation" localSheetId="1">BOM_PWMAttenuation!$A$1:$H$22</definedName>
+    <definedName name="PWMAttenuation" localSheetId="0">BOM_PSC!$A$1:$E$17</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
@@ -44,25 +42,11 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="2" name="PWMAttenuation1" type="6" refreshedVersion="5" background="1" saveData="1">
-    <textPr codePage="1250" sourceFile="C:\Users\kakareka\projects\PRiME\notes\Gen1\BOM\PWMAttenuation.csv" semicolon="1">
-      <textFields count="8">
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-      </textFields>
-    </textPr>
-  </connection>
 </connections>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="111">
   <si>
     <t>Qty</t>
   </si>
@@ -392,13 +376,16 @@
   </si>
   <si>
     <t>2-pin 3.5mm terminal block plug</t>
+  </si>
+  <si>
+    <t>PWMAttenuation</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -407,8 +394,24 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -423,7 +426,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor theme="4"/>
       </patternFill>
     </fill>
   </fills>
@@ -438,18 +441,37 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Neutral" xfId="1" builtinId="28"/>
+    <cellStyle name="Accent1" xfId="1" builtinId="29"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="2">
@@ -495,10 +517,6 @@
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PWMAttenuation" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PWMAttenuation" connectionId="2" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -764,601 +782,588 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D16"/>
+  <dimension ref="A1:G31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="81.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="37.7109375" customWidth="1"/>
+    <col min="1" max="1" width="4.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30" style="1" customWidth="1"/>
+    <col min="3" max="3" width="31.7109375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="15" style="1" customWidth="1"/>
+    <col min="5" max="5" width="66" style="2" customWidth="1"/>
+    <col min="6" max="6" width="49.7109375" style="1" customWidth="1"/>
+    <col min="7" max="7" width="36.85546875" style="1" customWidth="1"/>
+    <col min="8" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
         <v>1</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
         <v>2</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="1" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
         <v>8</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="1" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
         <v>2</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="1" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
         <v>1</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="1" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D12" s="2"/>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D15" s="2"/>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C16" s="1"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G22"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="4.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="81.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="37.7109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="3"/>
+      <c r="B8" s="3"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="4"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3"/>
+    </row>
+    <row r="9" spans="1:7" ht="21" x14ac:dyDescent="0.25">
+      <c r="B9" s="5" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B10" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C10" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D10" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E10" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F10" s="6" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B11" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C11" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D11" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E11" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F11" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G11" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3">
+    <row r="12" spans="1:7" ht="135" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
         <v>66</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B12" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C12" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D12" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E12" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F12" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="G3"/>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4">
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
         <v>8</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B13" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C13" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D13" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E13" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="F4" t="s">
+      <c r="F13" s="1" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
         <v>2</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B14" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C14" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D14" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E14" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="F5" t="s">
+      <c r="F14" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="G5" t="s">
+      <c r="G14" s="1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6">
+    <row r="15" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
         <v>8</v>
       </c>
-      <c r="B6">
+      <c r="B15" s="1">
         <v>100</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C15" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D15" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E15" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="F6" t="s">
+      <c r="F15" s="1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7">
+    <row r="16" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
         <v>24</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B16" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C16" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D16" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="E7" t="s">
+      <c r="E16" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="F7" t="s">
+      <c r="F16" s="1" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="1">
         <v>2</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B17" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C17" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D17" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="E8" t="s">
+      <c r="E17" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="F8" t="s">
+      <c r="F17" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="G8" t="s">
+      <c r="G17" s="1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="1">
         <v>1</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B18" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C18" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="D9">
+      <c r="D18" s="1">
         <v>1844210</v>
       </c>
-      <c r="E9" t="s">
+      <c r="E18" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="F9" t="s">
+      <c r="F18" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="G9" t="s">
+      <c r="G18" s="1" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="1">
         <v>1</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B19" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C19" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="D10">
+      <c r="D19" s="1">
         <v>1844265</v>
       </c>
-      <c r="E10" t="s">
+      <c r="E19" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="F10" t="s">
+      <c r="F19" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="G10" t="s">
+      <c r="G19" s="1" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="1">
         <v>1</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B20" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C20" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D20" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="E11" t="s">
+      <c r="E20" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="F11" t="s">
+      <c r="F20" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="G11" t="s">
+      <c r="G20" s="1" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="1">
         <v>3</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B21" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C21" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D21" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="E12" t="s">
+      <c r="E21" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="F12" t="s">
+      <c r="F21" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="G12" t="s">
+      <c r="G21" s="1" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13">
+    <row r="22" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A22" s="1">
         <v>16</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B22" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C22" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="D13" t="s">
+      <c r="D22" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="E13" t="s">
+      <c r="E22" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="F13" t="s">
+      <c r="F22" s="1" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14">
+    <row r="23" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A23" s="1">
         <v>32</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B23" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C23" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="D14" t="s">
+      <c r="D23" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="E14" t="s">
+      <c r="E23" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="F14" t="s">
+      <c r="F23" s="1" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" s="1">
         <v>2</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B24" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C24" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D15" t="s">
+      <c r="D24" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="E15" t="s">
+      <c r="E24" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="F15" t="s">
+      <c r="F24" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="G15" t="s">
+      <c r="G24" s="1" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" s="1">
         <v>8</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B25" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C25" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="D16" t="s">
+      <c r="D25" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="E16" t="s">
+      <c r="E25" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="F16" t="s">
+      <c r="F25" s="1" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" s="1">
         <v>1</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B26" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C26" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="D17">
+      <c r="D26" s="1">
         <v>1844359</v>
       </c>
-      <c r="E17" t="s">
+      <c r="E26" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="F17" t="s">
+      <c r="F26" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="G17" t="s">
+      <c r="G26" s="1" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" s="1">
         <v>1</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B27" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C27" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="D18" t="s">
+      <c r="D27" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="E18" t="s">
+      <c r="E27" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="F18" t="s">
+      <c r="F27" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="G18" s="2" t="s">
+      <c r="G27" s="8" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19">
+    <row r="28" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A28" s="1">
         <v>16</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B28" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C28" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="D19" t="s">
+      <c r="D28" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="E19" t="s">
+      <c r="E28" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="F19" t="s">
+      <c r="F28" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="G19" t="s">
+      <c r="G28" s="1" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" s="1">
         <v>8</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B29" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C29" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="D20" t="s">
+      <c r="D29" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="E20" t="s">
+      <c r="E29" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="F20" t="s">
+      <c r="F29" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="G20" t="s">
+      <c r="G29" s="1" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" s="1">
         <v>1</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B30" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C30" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="D21" t="s">
+      <c r="D30" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="E21" t="s">
+      <c r="E30" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="F21" t="s">
+      <c r="F30" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="G21" s="2" t="s">
+      <c r="G30" s="8" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" s="1">
         <v>1</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B31" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="C22" t="s">
+      <c r="C31" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="D22" t="s">
+      <c r="D31" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="E22" t="s">
+      <c r="E31" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="F22" t="s">
+      <c r="F31" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="G22" t="s">
+      <c r="G31" s="1" t="s">
         <v>98</v>
       </c>
     </row>

</xml_diff>